<commit_message>
P06 Task3 MICE & Emporium etc.
</commit_message>
<xml_diff>
--- a/P06/doc/Scrum_MICE_Sprint_2.xlsx
+++ b/P06/doc/Scrum_MICE_Sprint_2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" state="visible" r:id="rId2"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="191">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -623,6 +623,12 @@
   </si>
   <si>
     <t xml:space="preserve">Regression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git commit -m "P06 Task2 MICE &amp; Emporium"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git commit -m "P06 Task3 MICE &amp; Emporium etc."</t>
   </si>
   <si>
     <t xml:space="preserve">BONUS</t>
@@ -1040,7 +1046,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart43.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1198,11 +1204,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="88837802"/>
-        <c:axId val="66633543"/>
+        <c:axId val="3329387"/>
+        <c:axId val="80678032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="88837802"/>
+        <c:axId val="3329387"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1269,12 +1275,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66633543"/>
+        <c:crossAx val="80678032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66633543"/>
+        <c:axId val="80678032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1349,7 +1355,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88837802"/>
+        <c:crossAx val="3329387"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1376,7 +1382,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart44.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1504,11 +1510,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="55633128"/>
-        <c:axId val="81455343"/>
+        <c:axId val="52335263"/>
+        <c:axId val="51880895"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="55633128"/>
+        <c:axId val="52335263"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1573,7 +1579,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81455343"/>
+        <c:crossAx val="51880895"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1581,7 +1587,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81455343"/>
+        <c:axId val="51880895"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1655,7 +1661,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="55633128"/>
+        <c:crossAx val="52335263"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1682,7 +1688,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart45.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1774,28 +1780,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1810,11 +1816,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="73650899"/>
-        <c:axId val="93848875"/>
+        <c:axId val="25362544"/>
+        <c:axId val="59055670"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73650899"/>
+        <c:axId val="25362544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1879,7 +1885,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93848875"/>
+        <c:crossAx val="59055670"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1887,7 +1893,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93848875"/>
+        <c:axId val="59055670"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1961,7 +1967,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73650899"/>
+        <c:crossAx val="25362544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1988,7 +1994,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart46.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2116,11 +2122,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="56543527"/>
-        <c:axId val="51689397"/>
+        <c:axId val="52200657"/>
+        <c:axId val="32450008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="56543527"/>
+        <c:axId val="52200657"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2185,7 +2191,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51689397"/>
+        <c:crossAx val="32450008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2193,7 +2199,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51689397"/>
+        <c:axId val="32450008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2267,7 +2273,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56543527"/>
+        <c:crossAx val="52200657"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2294,7 +2300,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart47.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2422,11 +2428,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="31746581"/>
-        <c:axId val="99912109"/>
+        <c:axId val="87719445"/>
+        <c:axId val="99363889"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="31746581"/>
+        <c:axId val="87719445"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2491,7 +2497,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99912109"/>
+        <c:crossAx val="99363889"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2499,7 +2505,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99912109"/>
+        <c:axId val="99363889"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2573,7 +2579,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31746581"/>
+        <c:crossAx val="87719445"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2600,7 +2606,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart48.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2728,11 +2734,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="69621205"/>
-        <c:axId val="57389134"/>
+        <c:axId val="76913616"/>
+        <c:axId val="65234441"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="69621205"/>
+        <c:axId val="76913616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2797,7 +2803,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57389134"/>
+        <c:crossAx val="65234441"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2805,7 +2811,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57389134"/>
+        <c:axId val="65234441"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2879,7 +2885,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="69621205"/>
+        <c:crossAx val="76913616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2906,7 +2912,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart49.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3034,11 +3040,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="43491722"/>
-        <c:axId val="83030804"/>
+        <c:axId val="23393867"/>
+        <c:axId val="1421264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="43491722"/>
+        <c:axId val="23393867"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3103,7 +3109,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83030804"/>
+        <c:crossAx val="1421264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3111,7 +3117,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83030804"/>
+        <c:axId val="1421264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3185,7 +3191,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43491722"/>
+        <c:crossAx val="23393867"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3465,8 +3471,8 @@
   </sheetPr>
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C16" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5419,7 +5425,7 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
@@ -6504,8 +6510,8 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6597,7 +6603,7 @@
       </c>
       <c r="B7" s="21" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
@@ -6610,7 +6616,7 @@
       </c>
       <c r="B8" s="21" t="n">
         <f aca="false">B7-C8</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C8" s="21" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -6626,7 +6632,7 @@
       </c>
       <c r="B9" s="21" t="n">
         <f aca="false">B8-C9</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C9" s="21" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -6642,7 +6648,7 @@
       </c>
       <c r="B10" s="21" t="n">
         <f aca="false">B9-C10</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C10" s="21" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -6658,7 +6664,7 @@
       </c>
       <c r="B11" s="21" t="n">
         <f aca="false">B10-C11</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" s="21" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -6674,7 +6680,7 @@
       </c>
       <c r="B12" s="21" t="n">
         <f aca="false">B11-C12</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C12" s="21" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -6690,7 +6696,7 @@
       </c>
       <c r="B13" s="21" t="n">
         <f aca="false">B12-C13</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13" s="21" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -6706,7 +6712,7 @@
       </c>
       <c r="B14" s="21" t="n">
         <f aca="false">B13-C14</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C14" s="21" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -6748,7 +6754,12 @@
       <c r="A17" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B17" s="33"/>
+      <c r="B17" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>9</v>
+      </c>
       <c r="D17" s="31" t="s">
         <v>180</v>
       </c>
@@ -6758,664 +6769,763 @@
       <c r="A18" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B18" s="33"/>
-      <c r="D18" s="33"/>
+      <c r="B18" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>187</v>
+      </c>
       <c r="E18" s="32"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="D19" s="33"/>
+      <c r="B19" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>188</v>
+      </c>
       <c r="E19" s="32"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="D20" s="33"/>
+      <c r="B20" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="29"/>
       <c r="E20" s="32"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B21" s="33"/>
-      <c r="D21" s="33"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="29"/>
       <c r="E21" s="32"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B22" s="33"/>
-      <c r="D22" s="33"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="29"/>
       <c r="E22" s="32"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B23" s="33"/>
-      <c r="D23" s="33"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="29"/>
       <c r="E23" s="32"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="D24" s="33"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="29"/>
       <c r="E24" s="32"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="B25" s="33"/>
-      <c r="D25" s="33"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="29"/>
       <c r="E25" s="32"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B26" s="33"/>
-      <c r="D26" s="33"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="29"/>
       <c r="E26" s="32"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B27" s="33"/>
-      <c r="D27" s="33"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="29"/>
       <c r="E27" s="32"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="B28" s="33"/>
-      <c r="D28" s="33"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="29"/>
       <c r="E28" s="32"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="B29" s="33"/>
-      <c r="D29" s="33"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="29"/>
       <c r="E29" s="32"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="D30" s="33"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="29"/>
       <c r="E30" s="32"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="D31" s="33"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="29"/>
       <c r="E31" s="32"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="B32" s="33"/>
-      <c r="D32" s="33"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="29"/>
       <c r="E32" s="32"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B33" s="33"/>
-      <c r="D33" s="33"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="29"/>
       <c r="E33" s="32"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="B34" s="33"/>
-      <c r="D34" s="33"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="29"/>
       <c r="E34" s="32"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="B35" s="33"/>
-      <c r="D35" s="33"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="29"/>
       <c r="E35" s="32"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="B36" s="33"/>
-      <c r="D36" s="33"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="29"/>
       <c r="E36" s="32"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="B37" s="33"/>
-      <c r="D37" s="33"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="29"/>
       <c r="E37" s="32"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="B38" s="33"/>
-      <c r="D38" s="33"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="29"/>
       <c r="E38" s="32"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="B39" s="33"/>
-      <c r="D39" s="33"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="29"/>
       <c r="E39" s="32"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="B40" s="33"/>
-      <c r="D40" s="33"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="29"/>
       <c r="E40" s="32"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="B41" s="33"/>
-      <c r="D41" s="33"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="30"/>
+      <c r="D41" s="29"/>
       <c r="E41" s="32"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="B42" s="33"/>
-      <c r="D42" s="33"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="29"/>
       <c r="E42" s="32"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
         <v>27</v>
       </c>
-      <c r="B43" s="33"/>
-      <c r="D43" s="33"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="29"/>
       <c r="E43" s="32"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
         <v>28</v>
       </c>
-      <c r="B44" s="33"/>
-      <c r="D44" s="33"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="29"/>
       <c r="E44" s="32"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="B45" s="33"/>
-      <c r="D45" s="33"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="29"/>
       <c r="E45" s="32"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="B46" s="33"/>
-      <c r="D46" s="33"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="29"/>
       <c r="E46" s="32"/>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
         <v>31</v>
       </c>
-      <c r="B47" s="33"/>
-      <c r="D47" s="33"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="29"/>
       <c r="E47" s="32"/>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="B48" s="33"/>
-      <c r="D48" s="33"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="29"/>
       <c r="E48" s="32"/>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
         <v>33</v>
       </c>
-      <c r="B49" s="33"/>
-      <c r="D49" s="33"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="29"/>
       <c r="E49" s="32"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="B50" s="33"/>
-      <c r="D50" s="33"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="29"/>
       <c r="E50" s="32"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="B51" s="33"/>
-      <c r="D51" s="33"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="30"/>
+      <c r="D51" s="29"/>
       <c r="E51" s="32"/>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="B52" s="33"/>
-      <c r="D52" s="33"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="29"/>
       <c r="E52" s="32"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
         <v>37</v>
       </c>
-      <c r="B53" s="33"/>
-      <c r="D53" s="33"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="29"/>
       <c r="E53" s="32"/>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="B54" s="33"/>
-      <c r="D54" s="33"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="29"/>
       <c r="E54" s="32"/>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
         <v>39</v>
       </c>
-      <c r="B55" s="33"/>
-      <c r="D55" s="33"/>
+      <c r="B55" s="29"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="29"/>
       <c r="E55" s="32"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="B56" s="33"/>
-      <c r="D56" s="33"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="29"/>
       <c r="E56" s="32"/>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
         <v>41</v>
       </c>
-      <c r="B57" s="33"/>
-      <c r="D57" s="33"/>
+      <c r="B57" s="29"/>
+      <c r="C57" s="30"/>
+      <c r="D57" s="29"/>
       <c r="E57" s="32"/>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
         <v>42</v>
       </c>
-      <c r="B58" s="33"/>
-      <c r="D58" s="33"/>
+      <c r="B58" s="29"/>
+      <c r="C58" s="30"/>
+      <c r="D58" s="29"/>
       <c r="E58" s="32"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
         <v>43</v>
       </c>
-      <c r="B59" s="33"/>
-      <c r="D59" s="33"/>
+      <c r="B59" s="29"/>
+      <c r="C59" s="30"/>
+      <c r="D59" s="29"/>
       <c r="E59" s="32"/>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
         <v>44</v>
       </c>
-      <c r="B60" s="33"/>
-      <c r="D60" s="33"/>
+      <c r="B60" s="29"/>
+      <c r="C60" s="30"/>
+      <c r="D60" s="29"/>
       <c r="E60" s="32"/>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="B61" s="33"/>
-      <c r="D61" s="33"/>
+      <c r="B61" s="29"/>
+      <c r="C61" s="30"/>
+      <c r="D61" s="29"/>
       <c r="E61" s="32"/>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
         <v>46</v>
       </c>
-      <c r="B62" s="33"/>
-      <c r="D62" s="33"/>
+      <c r="B62" s="29"/>
+      <c r="C62" s="30"/>
+      <c r="D62" s="29"/>
       <c r="E62" s="32"/>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
         <v>47</v>
       </c>
-      <c r="B63" s="33"/>
-      <c r="D63" s="33"/>
+      <c r="B63" s="29"/>
+      <c r="C63" s="30"/>
+      <c r="D63" s="29"/>
       <c r="E63" s="32"/>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="B64" s="33"/>
-      <c r="D64" s="33"/>
+      <c r="B64" s="29"/>
+      <c r="C64" s="30"/>
+      <c r="D64" s="29"/>
       <c r="E64" s="32"/>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
         <v>49</v>
       </c>
-      <c r="B65" s="33"/>
-      <c r="D65" s="33"/>
+      <c r="B65" s="29"/>
+      <c r="C65" s="30"/>
+      <c r="D65" s="29"/>
       <c r="E65" s="32"/>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="B66" s="33"/>
-      <c r="D66" s="33"/>
+      <c r="B66" s="29"/>
+      <c r="C66" s="30"/>
+      <c r="D66" s="29"/>
       <c r="E66" s="32"/>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
         <v>51</v>
       </c>
-      <c r="B67" s="33"/>
-      <c r="D67" s="33"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="30"/>
+      <c r="D67" s="29"/>
       <c r="E67" s="32"/>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
         <v>52</v>
       </c>
-      <c r="B68" s="33"/>
-      <c r="D68" s="33"/>
+      <c r="B68" s="29"/>
+      <c r="C68" s="30"/>
+      <c r="D68" s="29"/>
       <c r="E68" s="32"/>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
         <v>53</v>
       </c>
-      <c r="B69" s="33"/>
-      <c r="D69" s="33"/>
+      <c r="B69" s="29"/>
+      <c r="C69" s="30"/>
+      <c r="D69" s="29"/>
       <c r="E69" s="32"/>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
         <v>54</v>
       </c>
-      <c r="B70" s="33"/>
-      <c r="D70" s="33"/>
+      <c r="B70" s="29"/>
+      <c r="C70" s="30"/>
+      <c r="D70" s="29"/>
       <c r="E70" s="32"/>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="B71" s="33"/>
-      <c r="D71" s="33"/>
+      <c r="B71" s="29"/>
+      <c r="C71" s="30"/>
+      <c r="D71" s="29"/>
       <c r="E71" s="32"/>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
         <v>56</v>
       </c>
-      <c r="B72" s="33"/>
-      <c r="D72" s="33"/>
+      <c r="B72" s="29"/>
+      <c r="C72" s="30"/>
+      <c r="D72" s="29"/>
       <c r="E72" s="32"/>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="B73" s="33"/>
-      <c r="D73" s="33"/>
+      <c r="B73" s="29"/>
+      <c r="C73" s="30"/>
+      <c r="D73" s="29"/>
       <c r="E73" s="32"/>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
         <v>58</v>
       </c>
-      <c r="B74" s="33"/>
-      <c r="D74" s="33"/>
+      <c r="B74" s="29"/>
+      <c r="C74" s="30"/>
+      <c r="D74" s="29"/>
       <c r="E74" s="32"/>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
         <v>59</v>
       </c>
-      <c r="B75" s="33"/>
-      <c r="D75" s="33"/>
+      <c r="B75" s="29"/>
+      <c r="C75" s="30"/>
+      <c r="D75" s="29"/>
       <c r="E75" s="32"/>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
         <v>60</v>
       </c>
-      <c r="B76" s="33"/>
-      <c r="D76" s="33"/>
+      <c r="B76" s="29"/>
+      <c r="C76" s="30"/>
+      <c r="D76" s="29"/>
       <c r="E76" s="32"/>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
         <v>61</v>
       </c>
-      <c r="B77" s="33"/>
-      <c r="D77" s="33"/>
+      <c r="B77" s="29"/>
+      <c r="C77" s="30"/>
+      <c r="D77" s="29"/>
       <c r="E77" s="32"/>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
         <v>62</v>
       </c>
-      <c r="B78" s="33"/>
-      <c r="D78" s="33"/>
+      <c r="B78" s="29"/>
+      <c r="C78" s="30"/>
+      <c r="D78" s="29"/>
       <c r="E78" s="32"/>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
         <v>63</v>
       </c>
-      <c r="B79" s="33"/>
-      <c r="D79" s="33"/>
+      <c r="B79" s="29"/>
+      <c r="C79" s="30"/>
+      <c r="D79" s="29"/>
       <c r="E79" s="32"/>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
         <v>64</v>
       </c>
-      <c r="B80" s="33"/>
-      <c r="D80" s="33"/>
+      <c r="B80" s="29"/>
+      <c r="C80" s="30"/>
+      <c r="D80" s="29"/>
       <c r="E80" s="32"/>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
         <v>65</v>
       </c>
-      <c r="B81" s="33"/>
-      <c r="D81" s="33"/>
+      <c r="B81" s="29"/>
+      <c r="C81" s="30"/>
+      <c r="D81" s="29"/>
       <c r="E81" s="32"/>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
         <v>66</v>
       </c>
-      <c r="B82" s="33"/>
-      <c r="D82" s="33"/>
+      <c r="B82" s="29"/>
+      <c r="C82" s="30"/>
+      <c r="D82" s="29"/>
       <c r="E82" s="32"/>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
         <v>67</v>
       </c>
-      <c r="B83" s="33"/>
-      <c r="D83" s="33"/>
+      <c r="B83" s="29"/>
+      <c r="C83" s="30"/>
+      <c r="D83" s="29"/>
       <c r="E83" s="32"/>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
         <v>68</v>
       </c>
-      <c r="B84" s="33"/>
-      <c r="D84" s="33"/>
+      <c r="B84" s="29"/>
+      <c r="C84" s="30"/>
+      <c r="D84" s="29"/>
       <c r="E84" s="32"/>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
         <v>69</v>
       </c>
-      <c r="B85" s="33"/>
-      <c r="D85" s="33"/>
+      <c r="B85" s="29"/>
+      <c r="C85" s="30"/>
+      <c r="D85" s="29"/>
       <c r="E85" s="32"/>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
         <v>70</v>
       </c>
-      <c r="B86" s="33"/>
-      <c r="D86" s="33"/>
+      <c r="B86" s="29"/>
+      <c r="C86" s="30"/>
+      <c r="D86" s="29"/>
       <c r="E86" s="32"/>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
         <v>71</v>
       </c>
-      <c r="B87" s="33"/>
-      <c r="D87" s="33"/>
+      <c r="B87" s="29"/>
+      <c r="C87" s="30"/>
+      <c r="D87" s="29"/>
       <c r="E87" s="32"/>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
         <v>72</v>
       </c>
-      <c r="B88" s="33"/>
-      <c r="D88" s="33"/>
+      <c r="B88" s="29"/>
+      <c r="C88" s="30"/>
+      <c r="D88" s="29"/>
       <c r="E88" s="32"/>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
         <v>73</v>
       </c>
-      <c r="B89" s="33"/>
-      <c r="D89" s="33"/>
+      <c r="B89" s="29"/>
+      <c r="C89" s="30"/>
+      <c r="D89" s="29"/>
       <c r="E89" s="32"/>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
         <v>74</v>
       </c>
-      <c r="B90" s="33"/>
-      <c r="D90" s="33"/>
+      <c r="B90" s="29"/>
+      <c r="C90" s="30"/>
+      <c r="D90" s="29"/>
       <c r="E90" s="32"/>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
         <v>75</v>
       </c>
-      <c r="B91" s="33"/>
-      <c r="D91" s="33"/>
+      <c r="B91" s="29"/>
+      <c r="C91" s="30"/>
+      <c r="D91" s="29"/>
       <c r="E91" s="32"/>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
         <v>76</v>
       </c>
-      <c r="B92" s="33"/>
-      <c r="D92" s="33"/>
+      <c r="B92" s="29"/>
+      <c r="C92" s="30"/>
+      <c r="D92" s="29"/>
       <c r="E92" s="32"/>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
         <v>77</v>
       </c>
-      <c r="B93" s="33"/>
-      <c r="D93" s="33"/>
+      <c r="B93" s="29"/>
+      <c r="C93" s="30"/>
+      <c r="D93" s="29"/>
       <c r="E93" s="32"/>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="n">
         <v>78</v>
       </c>
-      <c r="B94" s="33"/>
-      <c r="D94" s="33"/>
+      <c r="B94" s="29"/>
+      <c r="C94" s="30"/>
+      <c r="D94" s="29"/>
       <c r="E94" s="32"/>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="n">
         <v>79</v>
       </c>
-      <c r="B95" s="33"/>
-      <c r="D95" s="33"/>
+      <c r="B95" s="29"/>
+      <c r="C95" s="30"/>
+      <c r="D95" s="29"/>
       <c r="E95" s="32"/>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="B96" s="33"/>
-      <c r="D96" s="33"/>
+      <c r="B96" s="29"/>
+      <c r="C96" s="30"/>
+      <c r="D96" s="29"/>
       <c r="E96" s="32"/>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="n">
         <v>81</v>
       </c>
-      <c r="B97" s="33"/>
-      <c r="D97" s="33"/>
+      <c r="B97" s="29"/>
+      <c r="C97" s="30"/>
+      <c r="D97" s="29"/>
       <c r="E97" s="32"/>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="n">
         <v>82</v>
       </c>
-      <c r="B98" s="33"/>
-      <c r="D98" s="33"/>
+      <c r="B98" s="29"/>
+      <c r="C98" s="30"/>
+      <c r="D98" s="29"/>
       <c r="E98" s="32"/>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="n">
         <v>83</v>
       </c>
-      <c r="B99" s="33"/>
-      <c r="D99" s="33"/>
+      <c r="B99" s="29"/>
+      <c r="C99" s="30"/>
+      <c r="D99" s="29"/>
       <c r="E99" s="32"/>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="n">
         <v>84</v>
       </c>
-      <c r="B100" s="33"/>
-      <c r="D100" s="33"/>
+      <c r="B100" s="29"/>
+      <c r="C100" s="30"/>
+      <c r="D100" s="29"/>
       <c r="E100" s="32"/>
     </row>
   </sheetData>
@@ -10360,7 +10470,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>2</v>
@@ -10556,7 +10666,7 @@
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
       <c r="D15" s="21" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E15" s="21"/>
       <c r="F15" s="21"/>

</xml_diff>

<commit_message>
P06 Task3 MICE - GUI
</commit_message>
<xml_diff>
--- a/P06/doc/Scrum_MICE_Sprint_2.xlsx
+++ b/P06/doc/Scrum_MICE_Sprint_2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" state="visible" r:id="rId2"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="192">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -629,6 +629,9 @@
   </si>
   <si>
     <t xml:space="preserve">git commit -m "P06 Task3 MICE &amp; Emporium etc."</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git commit -m "P06 Task3 MICE – GUI"</t>
   </si>
   <si>
     <t xml:space="preserve">BONUS</t>
@@ -1046,7 +1049,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart64.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1204,11 +1207,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="3329387"/>
-        <c:axId val="80678032"/>
+        <c:axId val="41225297"/>
+        <c:axId val="24979986"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="3329387"/>
+        <c:axId val="41225297"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1275,12 +1278,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80678032"/>
+        <c:crossAx val="24979986"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80678032"/>
+        <c:axId val="24979986"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1355,7 +1358,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3329387"/>
+        <c:crossAx val="41225297"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1382,7 +1385,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart65.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1510,11 +1513,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="52335263"/>
-        <c:axId val="51880895"/>
+        <c:axId val="33996627"/>
+        <c:axId val="10707022"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="52335263"/>
+        <c:axId val="33996627"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1579,7 +1582,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51880895"/>
+        <c:crossAx val="10707022"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1587,7 +1590,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51880895"/>
+        <c:axId val="10707022"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1661,7 +1664,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52335263"/>
+        <c:crossAx val="33996627"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1688,7 +1691,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart66.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1780,28 +1783,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1816,11 +1819,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="25362544"/>
-        <c:axId val="59055670"/>
+        <c:axId val="66577142"/>
+        <c:axId val="19296992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="25362544"/>
+        <c:axId val="66577142"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1885,7 +1888,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59055670"/>
+        <c:crossAx val="19296992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1893,7 +1896,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59055670"/>
+        <c:axId val="19296992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1967,7 +1970,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25362544"/>
+        <c:crossAx val="66577142"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1994,7 +1997,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart67.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2122,11 +2125,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="52200657"/>
-        <c:axId val="32450008"/>
+        <c:axId val="84791176"/>
+        <c:axId val="89903919"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="52200657"/>
+        <c:axId val="84791176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2191,7 +2194,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32450008"/>
+        <c:crossAx val="89903919"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2199,7 +2202,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="32450008"/>
+        <c:axId val="89903919"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2273,7 +2276,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52200657"/>
+        <c:crossAx val="84791176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2300,7 +2303,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart68.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2428,11 +2431,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="87719445"/>
-        <c:axId val="99363889"/>
+        <c:axId val="18650272"/>
+        <c:axId val="87043893"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="87719445"/>
+        <c:axId val="18650272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2497,7 +2500,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99363889"/>
+        <c:crossAx val="87043893"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2505,7 +2508,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99363889"/>
+        <c:axId val="87043893"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2579,7 +2582,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87719445"/>
+        <c:crossAx val="18650272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2606,7 +2609,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart69.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2734,11 +2737,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="76913616"/>
-        <c:axId val="65234441"/>
+        <c:axId val="81721516"/>
+        <c:axId val="50202176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="76913616"/>
+        <c:axId val="81721516"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2803,7 +2806,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65234441"/>
+        <c:crossAx val="50202176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2811,7 +2814,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65234441"/>
+        <c:axId val="50202176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2885,7 +2888,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76913616"/>
+        <c:crossAx val="81721516"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2912,7 +2915,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart49.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart70.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3040,11 +3043,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="23393867"/>
-        <c:axId val="1421264"/>
+        <c:axId val="48293932"/>
+        <c:axId val="40949766"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="23393867"/>
+        <c:axId val="48293932"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3109,7 +3112,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1421264"/>
+        <c:crossAx val="40949766"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3117,7 +3120,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1421264"/>
+        <c:axId val="40949766"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3191,7 +3194,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23393867"/>
+        <c:crossAx val="48293932"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3471,7 +3474,7 @@
   </sheetPr>
   <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
@@ -5425,8 +5428,8 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D25" activeCellId="0" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6510,8 +6513,8 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6603,7 +6606,7 @@
       </c>
       <c r="B7" s="21" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
@@ -6616,7 +6619,7 @@
       </c>
       <c r="B8" s="21" t="n">
         <f aca="false">B7-C8</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8" s="21" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -6632,7 +6635,7 @@
       </c>
       <c r="B9" s="21" t="n">
         <f aca="false">B8-C9</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9" s="21" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -6648,7 +6651,7 @@
       </c>
       <c r="B10" s="21" t="n">
         <f aca="false">B9-C10</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C10" s="21" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -6664,7 +6667,7 @@
       </c>
       <c r="B11" s="21" t="n">
         <f aca="false">B10-C11</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" s="21" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -6680,7 +6683,7 @@
       </c>
       <c r="B12" s="21" t="n">
         <f aca="false">B11-C12</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12" s="21" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -6696,7 +6699,7 @@
       </c>
       <c r="B13" s="21" t="n">
         <f aca="false">B12-C13</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" s="21" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -6712,7 +6715,7 @@
       </c>
       <c r="B14" s="21" t="n">
         <f aca="false">B13-C14</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C14" s="21" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -6805,7 +6808,9 @@
       <c r="C20" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="29"/>
+      <c r="D20" s="29" t="s">
+        <v>189</v>
+      </c>
       <c r="E20" s="32"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10470,7 +10475,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>2</v>
@@ -10666,7 +10671,7 @@
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
       <c r="D15" s="21" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E15" s="21"/>
       <c r="F15" s="21"/>

</xml_diff>